<commit_message>
update 2023-11-10 10:30:27 by desktop-stc66qq
</commit_message>
<xml_diff>
--- a/config/RNP_CTLConfig.xlsx
+++ b/config/RNP_CTLConfig.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20338"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4EE8B97F-C981-449C-98A3-E8DC6AD1BBA2}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{919BD85B-0114-4162-B753-1CD05D3BF1C5}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="13800" windowHeight="4392" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="13800" windowHeight="4395" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="2" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="446" uniqueCount="182">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="531" uniqueCount="191">
   <si>
     <t>paradigm</t>
   </si>
@@ -684,10 +684,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>1,2,3,4,5,6,7,8,9,10</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>#FF0000, #0000FF, #008000, #FFA500, #800080, #00FFFF,#FFC0CB, #4B0082,#FFD700,#C0C0C0</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -725,6 +721,46 @@
   </si>
   <si>
     <t>2o02,2o02,2o02,2o02,2o02,4o04,4o04,4o04,4o04,4o04</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1,2,3,4,5;6,7,8,9,10</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Anesthesia_Ratio_4_0512345_00</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>reg4-4.4,reg4-4.8,reg4-5.2,reg4-5.6,reg4-6,reg4-4.2</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>2001.9251,2001.9251,2001.9251,2001.9251,2001.9251,2001.9251</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>4,4,4,4,4,4</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>4.4,4.8,5.2,5.6,6,4.2</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Anesthesia_Ratio_4_0512345_20</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Anesthesia_Ratio_4_0512345_40</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Anesthesia_Ratio_4_0512345_80</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Anesthesia_Ratio_4_0512345_000</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -835,7 +871,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="2"/>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
@@ -892,6 +928,18 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
@@ -1173,38 +1221,38 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C23A6ACB-7C6B-4CD1-9AC1-822BCA547FA6}">
-  <dimension ref="A1:U26"/>
+  <dimension ref="A1:U32"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="M1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A14" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="L31" sqref="L31"/>
+    <sheetView tabSelected="1" topLeftCell="I1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A23" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A33" sqref="A33"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="50.33203125" style="1" customWidth="1"/>
-    <col min="2" max="2" width="52.109375" style="1" customWidth="1"/>
-    <col min="3" max="3" width="42.88671875" style="4" customWidth="1"/>
-    <col min="4" max="4" width="44.109375" style="4" customWidth="1"/>
-    <col min="5" max="5" width="40.33203125" style="4" customWidth="1"/>
-    <col min="6" max="7" width="14.6640625" style="1" customWidth="1"/>
-    <col min="8" max="8" width="20.77734375" style="4" customWidth="1"/>
-    <col min="9" max="9" width="11.44140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="50.375" style="1" customWidth="1"/>
+    <col min="2" max="2" width="52.125" style="1" customWidth="1"/>
+    <col min="3" max="3" width="42.875" style="4" customWidth="1"/>
+    <col min="4" max="4" width="43.875" style="4" customWidth="1"/>
+    <col min="5" max="5" width="43.5" style="4" customWidth="1"/>
+    <col min="6" max="7" width="14.625" style="1" customWidth="1"/>
+    <col min="8" max="8" width="20.75" style="4" customWidth="1"/>
+    <col min="9" max="9" width="11.5" style="1" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="23" style="4" customWidth="1"/>
-    <col min="11" max="11" width="23.44140625" style="4" customWidth="1"/>
-    <col min="12" max="12" width="87.88671875" customWidth="1"/>
-    <col min="13" max="13" width="9.6640625" customWidth="1"/>
-    <col min="14" max="14" width="10.77734375" customWidth="1"/>
-    <col min="15" max="15" width="15.88671875" style="1" customWidth="1"/>
-    <col min="16" max="16" width="15.88671875" customWidth="1"/>
-    <col min="17" max="17" width="15.88671875" style="1" customWidth="1"/>
+    <col min="11" max="11" width="23.5" style="4" customWidth="1"/>
+    <col min="12" max="12" width="87.875" customWidth="1"/>
+    <col min="13" max="13" width="9.625" customWidth="1"/>
+    <col min="14" max="14" width="10.75" customWidth="1"/>
+    <col min="15" max="15" width="15.875" style="1" customWidth="1"/>
+    <col min="16" max="16" width="15.875" customWidth="1"/>
+    <col min="17" max="17" width="15.875" style="1" customWidth="1"/>
     <col min="18" max="18" width="15" style="1" customWidth="1"/>
     <col min="19" max="19" width="20" style="8" customWidth="1"/>
     <col min="20" max="20" width="13" style="8" customWidth="1"/>
-    <col min="21" max="21" width="31.109375" style="1" customWidth="1"/>
+    <col min="21" max="21" width="31.125" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" s="14" customFormat="1" ht="27.6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:21" s="14" customFormat="1" ht="28.5" x14ac:dyDescent="0.2">
       <c r="A1" s="9" t="s">
         <v>0</v>
       </c>
@@ -1269,7 +1317,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="2" spans="1:21" s="14" customFormat="1" ht="69" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:21" s="14" customFormat="1" ht="71.25" x14ac:dyDescent="0.2">
       <c r="A2" s="16" t="s">
         <v>52</v>
       </c>
@@ -1300,7 +1348,7 @@
       </c>
       <c r="U2" s="12"/>
     </row>
-    <row r="3" spans="1:21" ht="41.4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:21" ht="28.5" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>108</v>
       </c>
@@ -1365,7 +1413,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="4" spans="1:21" ht="27.6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:21" ht="28.5" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>130</v>
       </c>
@@ -1430,7 +1478,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="5" spans="1:21" ht="27.6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:21" ht="28.5" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>109</v>
       </c>
@@ -1495,7 +1543,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="6" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
         <v>131</v>
       </c>
@@ -1560,7 +1608,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="7" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
         <v>110</v>
       </c>
@@ -1625,7 +1673,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="8" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
         <v>132</v>
       </c>
@@ -1690,7 +1738,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="9" spans="1:21" ht="27.6" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:21" ht="28.5" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
         <v>111</v>
       </c>
@@ -1755,7 +1803,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="10" spans="1:21" ht="27.6" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:21" ht="28.5" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
         <v>112</v>
       </c>
@@ -1820,7 +1868,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="11" spans="1:21" ht="27.6" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:21" ht="28.5" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
         <v>39</v>
       </c>
@@ -1885,7 +1933,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="12" spans="1:21" ht="27.6" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:21" ht="28.5" x14ac:dyDescent="0.2">
       <c r="A12" s="25" t="s">
         <v>104</v>
       </c>
@@ -1950,7 +1998,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="13" spans="1:21" ht="41.4" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:21" ht="42.75" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
         <v>44</v>
       </c>
@@ -2015,7 +2063,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="14" spans="1:21" ht="41.4" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:21" ht="42.75" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
         <v>55</v>
       </c>
@@ -2080,7 +2128,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="15" spans="1:21" ht="41.4" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:21" ht="42.75" x14ac:dyDescent="0.2">
       <c r="A15" s="1" t="s">
         <v>99</v>
       </c>
@@ -2145,7 +2193,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="16" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A16" s="27" t="s">
         <v>137</v>
       </c>
@@ -2208,7 +2256,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="17" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A17" s="1" t="s">
         <v>140</v>
       </c>
@@ -2270,7 +2318,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="18" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A18" s="1" t="s">
         <v>141</v>
       </c>
@@ -2332,7 +2380,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="19" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A19" s="27" t="s">
         <v>142</v>
       </c>
@@ -2394,7 +2442,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="20" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A20" s="27" t="s">
         <v>143</v>
       </c>
@@ -2456,7 +2504,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="21" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A21" s="27" t="s">
         <v>164</v>
       </c>
@@ -2518,7 +2566,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="22" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A22" s="1" t="s">
         <v>165</v>
       </c>
@@ -2580,7 +2628,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="23" spans="1:21" ht="41.4" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:21" ht="28.5" x14ac:dyDescent="0.2">
       <c r="A23" s="27" t="s">
         <v>168</v>
       </c>
@@ -2588,10 +2636,10 @@
         <v>169</v>
       </c>
       <c r="D23" s="4" t="s">
+        <v>178</v>
+      </c>
+      <c r="E23" s="4" t="s">
         <v>179</v>
-      </c>
-      <c r="E23" s="4" t="s">
-        <v>180</v>
       </c>
       <c r="F23" s="1" t="s">
         <v>58</v>
@@ -2609,10 +2657,10 @@
         <v>170</v>
       </c>
       <c r="K23" s="4" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="L23" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="M23" s="6">
         <v>0</v>
@@ -2624,7 +2672,7 @@
         <v>58</v>
       </c>
       <c r="P23" s="6" t="s">
-        <v>171</v>
+        <v>181</v>
       </c>
       <c r="Q23" s="1" t="s">
         <v>25</v>
@@ -2633,27 +2681,27 @@
         <v>8</v>
       </c>
       <c r="S23" s="8" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="T23" s="8" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="U23" s="1" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="24" spans="1:21" ht="27.6" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:21" ht="28.5" x14ac:dyDescent="0.2">
       <c r="A24" s="27" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="C24" s="3" t="s">
         <v>169</v>
       </c>
       <c r="D24" s="4" t="s">
+        <v>178</v>
+      </c>
+      <c r="E24" s="4" t="s">
         <v>179</v>
-      </c>
-      <c r="E24" s="4" t="s">
-        <v>180</v>
       </c>
       <c r="F24" s="1" t="s">
         <v>58</v>
@@ -2671,10 +2719,10 @@
         <v>170</v>
       </c>
       <c r="K24" s="4" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="L24" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="M24" s="6">
         <v>0</v>
@@ -2686,7 +2734,7 @@
         <v>58</v>
       </c>
       <c r="P24" s="6" t="s">
-        <v>171</v>
+        <v>181</v>
       </c>
       <c r="Q24" s="1" t="s">
         <v>25</v>
@@ -2695,27 +2743,27 @@
         <v>8</v>
       </c>
       <c r="S24" s="8" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="T24" s="8" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="U24" s="1" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="25" spans="1:21" ht="27.6" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:21" ht="28.5" x14ac:dyDescent="0.2">
       <c r="A25" s="27" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="C25" s="3" t="s">
         <v>169</v>
       </c>
       <c r="D25" s="4" t="s">
+        <v>178</v>
+      </c>
+      <c r="E25" s="4" t="s">
         <v>179</v>
-      </c>
-      <c r="E25" s="4" t="s">
-        <v>180</v>
       </c>
       <c r="F25" s="1" t="s">
         <v>58</v>
@@ -2733,10 +2781,10 @@
         <v>170</v>
       </c>
       <c r="K25" s="4" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="L25" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="M25" s="6">
         <v>0</v>
@@ -2748,7 +2796,7 @@
         <v>58</v>
       </c>
       <c r="P25" s="6" t="s">
-        <v>171</v>
+        <v>181</v>
       </c>
       <c r="Q25" s="1" t="s">
         <v>25</v>
@@ -2757,27 +2805,27 @@
         <v>8</v>
       </c>
       <c r="S25" s="8" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="T25" s="8" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="U25" s="1" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="26" spans="1:21" ht="27.6" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:21" ht="28.5" x14ac:dyDescent="0.2">
       <c r="A26" s="27" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="C26" s="3" t="s">
         <v>169</v>
       </c>
       <c r="D26" s="4" t="s">
+        <v>178</v>
+      </c>
+      <c r="E26" s="4" t="s">
         <v>179</v>
-      </c>
-      <c r="E26" s="4" t="s">
-        <v>180</v>
       </c>
       <c r="F26" s="1" t="s">
         <v>58</v>
@@ -2795,10 +2843,10 @@
         <v>170</v>
       </c>
       <c r="K26" s="4" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="L26" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="M26" s="6">
         <v>0</v>
@@ -2810,7 +2858,7 @@
         <v>58</v>
       </c>
       <c r="P26" s="6" t="s">
-        <v>171</v>
+        <v>181</v>
       </c>
       <c r="Q26" s="1" t="s">
         <v>25</v>
@@ -2819,12 +2867,327 @@
         <v>8</v>
       </c>
       <c r="S26" s="8" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="T26" s="8" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="U26" s="1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="28" spans="1:21" s="31" customFormat="1" ht="28.5" x14ac:dyDescent="0.2">
+      <c r="A28" s="28" t="s">
+        <v>182</v>
+      </c>
+      <c r="B28" s="28"/>
+      <c r="C28" s="29" t="s">
+        <v>183</v>
+      </c>
+      <c r="D28" s="29" t="s">
+        <v>184</v>
+      </c>
+      <c r="E28" s="29" t="s">
+        <v>184</v>
+      </c>
+      <c r="F28" s="28" t="s">
+        <v>58</v>
+      </c>
+      <c r="G28" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="H28" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="I28" s="29" t="s">
+        <v>10</v>
+      </c>
+      <c r="J28" s="28" t="s">
+        <v>185</v>
+      </c>
+      <c r="K28" s="29" t="s">
+        <v>186</v>
+      </c>
+      <c r="L28" s="29" t="s">
+        <v>167</v>
+      </c>
+      <c r="M28" s="28">
+        <v>0</v>
+      </c>
+      <c r="N28" s="28">
+        <v>6</v>
+      </c>
+      <c r="O28" s="28" t="s">
+        <v>58</v>
+      </c>
+      <c r="P28" s="28" t="s">
+        <v>75</v>
+      </c>
+      <c r="Q28" s="28" t="s">
+        <v>25</v>
+      </c>
+      <c r="R28" s="28">
+        <v>8</v>
+      </c>
+      <c r="S28" s="30" t="s">
+        <v>27</v>
+      </c>
+      <c r="T28" s="28" t="s">
+        <v>27</v>
+      </c>
+      <c r="U28" s="28" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="29" spans="1:21" s="31" customFormat="1" ht="28.5" x14ac:dyDescent="0.2">
+      <c r="A29" s="28" t="s">
+        <v>187</v>
+      </c>
+      <c r="B29" s="28"/>
+      <c r="C29" s="29" t="s">
+        <v>183</v>
+      </c>
+      <c r="D29" s="29" t="s">
+        <v>184</v>
+      </c>
+      <c r="E29" s="29" t="s">
+        <v>184</v>
+      </c>
+      <c r="F29" s="28" t="s">
+        <v>58</v>
+      </c>
+      <c r="G29" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="H29" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="I29" s="29" t="s">
+        <v>10</v>
+      </c>
+      <c r="J29" s="28" t="s">
+        <v>185</v>
+      </c>
+      <c r="K29" s="29" t="s">
+        <v>186</v>
+      </c>
+      <c r="L29" s="29" t="s">
+        <v>167</v>
+      </c>
+      <c r="M29" s="28">
+        <v>0</v>
+      </c>
+      <c r="N29" s="28">
+        <v>6</v>
+      </c>
+      <c r="O29" s="28" t="s">
+        <v>58</v>
+      </c>
+      <c r="P29" s="28" t="s">
+        <v>75</v>
+      </c>
+      <c r="Q29" s="28" t="s">
+        <v>25</v>
+      </c>
+      <c r="R29" s="28">
+        <v>8</v>
+      </c>
+      <c r="S29" s="30" t="s">
+        <v>27</v>
+      </c>
+      <c r="T29" s="28" t="s">
+        <v>27</v>
+      </c>
+      <c r="U29" s="28" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="30" spans="1:21" s="31" customFormat="1" ht="28.5" x14ac:dyDescent="0.2">
+      <c r="A30" s="28" t="s">
+        <v>188</v>
+      </c>
+      <c r="B30" s="28"/>
+      <c r="C30" s="29" t="s">
+        <v>183</v>
+      </c>
+      <c r="D30" s="29" t="s">
+        <v>184</v>
+      </c>
+      <c r="E30" s="29" t="s">
+        <v>184</v>
+      </c>
+      <c r="F30" s="28" t="s">
+        <v>58</v>
+      </c>
+      <c r="G30" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="H30" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="I30" s="29" t="s">
+        <v>10</v>
+      </c>
+      <c r="J30" s="28" t="s">
+        <v>185</v>
+      </c>
+      <c r="K30" s="29" t="s">
+        <v>186</v>
+      </c>
+      <c r="L30" s="29" t="s">
+        <v>167</v>
+      </c>
+      <c r="M30" s="28">
+        <v>0</v>
+      </c>
+      <c r="N30" s="28">
+        <v>6</v>
+      </c>
+      <c r="O30" s="28" t="s">
+        <v>58</v>
+      </c>
+      <c r="P30" s="28" t="s">
+        <v>75</v>
+      </c>
+      <c r="Q30" s="28" t="s">
+        <v>25</v>
+      </c>
+      <c r="R30" s="28">
+        <v>8</v>
+      </c>
+      <c r="S30" s="30" t="s">
+        <v>27</v>
+      </c>
+      <c r="T30" s="28" t="s">
+        <v>27</v>
+      </c>
+      <c r="U30" s="28" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="31" spans="1:21" s="31" customFormat="1" ht="28.5" x14ac:dyDescent="0.2">
+      <c r="A31" s="28" t="s">
+        <v>189</v>
+      </c>
+      <c r="B31" s="28"/>
+      <c r="C31" s="29" t="s">
+        <v>183</v>
+      </c>
+      <c r="D31" s="29" t="s">
+        <v>184</v>
+      </c>
+      <c r="E31" s="29" t="s">
+        <v>184</v>
+      </c>
+      <c r="F31" s="28" t="s">
+        <v>58</v>
+      </c>
+      <c r="G31" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="H31" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="I31" s="29" t="s">
+        <v>10</v>
+      </c>
+      <c r="J31" s="28" t="s">
+        <v>185</v>
+      </c>
+      <c r="K31" s="29" t="s">
+        <v>186</v>
+      </c>
+      <c r="L31" s="29" t="s">
+        <v>167</v>
+      </c>
+      <c r="M31" s="28">
+        <v>0</v>
+      </c>
+      <c r="N31" s="28">
+        <v>6</v>
+      </c>
+      <c r="O31" s="28" t="s">
+        <v>58</v>
+      </c>
+      <c r="P31" s="28" t="s">
+        <v>75</v>
+      </c>
+      <c r="Q31" s="28" t="s">
+        <v>25</v>
+      </c>
+      <c r="R31" s="28">
+        <v>8</v>
+      </c>
+      <c r="S31" s="30" t="s">
+        <v>27</v>
+      </c>
+      <c r="T31" s="28" t="s">
+        <v>27</v>
+      </c>
+      <c r="U31" s="28" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="32" spans="1:21" s="31" customFormat="1" ht="28.5" x14ac:dyDescent="0.2">
+      <c r="A32" s="28" t="s">
+        <v>190</v>
+      </c>
+      <c r="B32" s="28"/>
+      <c r="C32" s="29" t="s">
+        <v>183</v>
+      </c>
+      <c r="D32" s="29" t="s">
+        <v>184</v>
+      </c>
+      <c r="E32" s="29" t="s">
+        <v>184</v>
+      </c>
+      <c r="F32" s="28" t="s">
+        <v>58</v>
+      </c>
+      <c r="G32" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="H32" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="I32" s="29" t="s">
+        <v>10</v>
+      </c>
+      <c r="J32" s="28" t="s">
+        <v>185</v>
+      </c>
+      <c r="K32" s="29" t="s">
+        <v>186</v>
+      </c>
+      <c r="L32" s="29" t="s">
+        <v>167</v>
+      </c>
+      <c r="M32" s="28">
+        <v>0</v>
+      </c>
+      <c r="N32" s="28">
+        <v>6</v>
+      </c>
+      <c r="O32" s="28" t="s">
+        <v>58</v>
+      </c>
+      <c r="P32" s="28" t="s">
+        <v>75</v>
+      </c>
+      <c r="Q32" s="28" t="s">
+        <v>25</v>
+      </c>
+      <c r="R32" s="28">
+        <v>8</v>
+      </c>
+      <c r="S32" s="30" t="s">
+        <v>27</v>
+      </c>
+      <c r="T32" s="28" t="s">
+        <v>27</v>
+      </c>
+      <c r="U32" s="28" t="s">
         <v>31</v>
       </c>
     </row>

</xml_diff>

<commit_message>
update 2025-05-05 16:16:00 by administrator
</commit_message>
<xml_diff>
--- a/config/RNP_CTLConfig.xlsx
+++ b/config/RNP_CTLConfig.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20338"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C20E38DA-CFEC-494F-917B-80F621D4B19A}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{09E60E29-7D39-4219-9DE1-4B365E37AC7A}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="13800" windowHeight="4395" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1191" uniqueCount="376">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1211" uniqueCount="378">
   <si>
     <t>paradigm</t>
   </si>
@@ -1472,6 +1472,14 @@
   </si>
   <si>
     <t>Recover_LocalGlobal_Only_4_5</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>LocalGlobal_Long_4_5</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Reg4-5(0),Reg4-5(1),Reg4-5(2),Reg4-5(4),Reg4-5(8),Reg4-5(16),Reg4-5(32),Reg4-5(Inf),Reg5-4(0),Reg5-4(1),Reg5-4(2),Reg5-4(4),Reg5-4(8),Reg5-4(16),Reg5-4(32),Reg5-4(Inf)</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -1590,7 +1598,7 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="2"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="2"/>
   </cellStyleXfs>
-  <cellXfs count="41">
+  <cellXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
@@ -1678,6 +1686,7 @@
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="9" applyFont="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="10">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
@@ -1967,11 +1976,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C23A6ACB-7C6B-4CD1-9AC1-822BCA547FA6}">
-  <dimension ref="A1:AA69"/>
+  <dimension ref="A1:AA70"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A62" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A70" sqref="A70"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A65" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="Z69" sqref="Z69"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -6271,6 +6280,74 @@
       <c r="Z69" s="8"/>
       <c r="AA69" s="1"/>
     </row>
+    <row r="70" spans="1:27" ht="42.75" x14ac:dyDescent="0.2">
+      <c r="A70" s="41" t="s">
+        <v>376</v>
+      </c>
+      <c r="C70" s="4" t="s">
+        <v>377</v>
+      </c>
+      <c r="D70" s="4" t="s">
+        <v>363</v>
+      </c>
+      <c r="E70" s="4" t="s">
+        <v>364</v>
+      </c>
+      <c r="F70" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="G70" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="H70" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="I70" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="J70" s="4" t="s">
+        <v>365</v>
+      </c>
+      <c r="K70" s="4" t="s">
+        <v>365</v>
+      </c>
+      <c r="L70" t="s">
+        <v>366</v>
+      </c>
+      <c r="M70" s="4" t="s">
+        <v>262</v>
+      </c>
+      <c r="N70" s="4" t="s">
+        <v>204</v>
+      </c>
+      <c r="O70" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="P70" s="6" t="s">
+        <v>367</v>
+      </c>
+      <c r="Q70" s="1" t="s">
+        <v>302</v>
+      </c>
+      <c r="R70" s="1" t="s">
+        <v>304</v>
+      </c>
+      <c r="S70" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="T70" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="U70" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="V70" s="1"/>
+      <c r="W70" s="1"/>
+      <c r="X70" s="6"/>
+      <c r="Y70" s="8"/>
+      <c r="Z70" s="8"/>
+      <c r="AA70" s="1"/>
+    </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
update 2025-11-22 11:25:19 by win-g08qkcqo325
</commit_message>
<xml_diff>
--- a/config/RNP_CTLConfig.xlsx
+++ b/config/RNP_CTLConfig.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20338"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24334"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{09E60E29-7D39-4219-9DE1-4B365E37AC7A}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F871CFE6-0151-43E7-8CA5-B8E690D53062}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="13800" windowHeight="4395" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="2" r:id="rId1"/>
@@ -15,12 +15,15 @@
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
+    <ext xmlns:xlwcv="http://schemas.microsoft.com/office/spreadsheetml/2024/workbookCompatibilityVersion" uri="{D14903EA-33C4-47F7-8F05-3474C54BE107}">
+      <xlwcv:version setVersion="1"/>
+    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1211" uniqueCount="378">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1410" uniqueCount="440">
   <si>
     <t>paradigm</t>
   </si>
@@ -1481,6 +1484,237 @@
   <si>
     <t>Reg4-5(0),Reg4-5(1),Reg4-5(2),Reg4-5(4),Reg4-5(8),Reg4-5(16),Reg4-5(32),Reg4-5(Inf),Reg5-4(0),Reg5-4(1),Reg5-4(2),Reg5-4(4),Reg5-4(8),Reg5-4(16),Reg5-4(32),Reg5-4(Inf)</t>
     <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Reflection_Regular</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Reflection_Irregular</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Level0-Control,Level0-Diff1,Level0-Diff2,Level0-Diff3,Level0-Diff4,Level1-Control,Level1-Diff1,Level1-Diff2,Level1-Diff3,Level1-Diff4,Level2-Control,Level2-Diff1,Level2-Diff2,Level2-Diff3,Level2-Diff4</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1000.9,1000.9,1000.9,1000.9,1000.9,1000.9,1000.9,1000.9,1000.9,1000.9,1000.9,1000.9,1000.9,1000.9,1000.9</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>2000,2000,2000,2000,2000,2000,2000,2000,2000,2000,2000,2000,2000,2000,2000</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>4,4,4,4,4,4,4,4,4,4,4,4,4,4,4</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>#AAAAAA,#000000,#0000FF,#FFA500,#FF0000,</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1,2,3,4,5;6,7,8,9,10;11,12,13,14,15</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1000.0102,1000.0102,1000.0102,1000.0102,1000.0102,1000.0102,1000.0102,1000.0102,1000.0102,1000.0102,1000.0102,1000.0102,1000.0102,1000.0102,1000.0102</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>LocalGlobal_IntControl</t>
+  </si>
+  <si>
+    <t>Insert32_0.8_0.2_0.5</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>2000</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>3000</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>4</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>#FF0000</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>LocalProcessing</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>f2000ICI5,f2025ICI5,f2050ICI5,f2075ICI5,f2100ICI5,f2125ICI5,f2000ICI25,f2025ICI25,f2050ICI25,f2075ICI25,f2100ICI25,f2125ICI25,f2000ICI125,f2025ICI125,f2050ICI125,f2075ICI125,f2100ICI125,f2125ICI125,f2000TB,f2025TB,f2050TB,f2075TB,f2100TB,F2125tb</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>2000,2000,2000,2000,2000,2000,2000,2000,2000,2000,2000,2000,2000,2000,2000,2000,2000,2000,2000,2000,2000,2000,2000,2000</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>5,5,5,5,5,5,25,25,25,25,25,25,125,125,125,125,125,125,1000,1000,1000,1000,1000,1000</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>#AAAAAA,#000000,#00FFFF,#0000FF,#FFA500,#FF0000</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1,2,3,4,5,6;7,8,9,10,11,12;13,14,15,16,17,18;19,20,21,22,23,24</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>f2000MT,f2025MT,f2050MT,f2075MT,f2075In1,f2075In5,f2075In25,f2075In125,f2075Alt,f2150MT,f2075MT2,f2000Reg,f2025Reg,f2050Reg,f2075Reg,f2000Irreg,f2025Irreg,f2050Irreg,f2075Irreg</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>#000000,#0000FF,#FFA500,#FF0000</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1,2,3,4;5,6,7,8;9,10,11;12,13,14,15;16,17,18,19</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Local_Process</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Rat_Offset_DiffICI</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1ms,2ms,4ms,8ms,16ms,32ms,64ms,128ms, noise</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>2560,2560,2560,2560,2560,2560,2560,2560,2560</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>-3000,1000</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>-3000,-200_9:-500,0</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1,2,3,4,5;5,6,7,8,9</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>16ms,48ms,144ms,432ms,1296ms,2500ms</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>2500,2500,2500,2500,2500,2500</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>#FF0000, #FFA500, #0000FF, #00FFFF,#000000, #AAAAAA</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1click,2click,4click,8click,16click,32click,64click,128click,256click,512click</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">0.01,4.01,12.02,28.04,60.07,124.13,252.25,508.50,1020.99,508,1020,2044  </t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>-3000,1500</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>-3000,1200</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>4,4,4,4,4,4,4,4,4,4</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>4,4,4,4,4,4,4,4,4,4</t>
+  </si>
+  <si>
+    <t>Rat_Offset_DiffDur</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Local_Process_New</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>f2000MT,f2025MT,f2050MT,f2075MT,f2075In1,f2075In5,f2075In25,f2075In125,f2000DurCtrl,f2075Dur2ms,f2075Dur6ms,f2075Dur18ms,f2150MT,f2075MT2,f2000Reg,f2025Reg,f2050Reg,f2075Reg,f2000Irreg,f2025Irreg,f2050Irreg,f2075Irreg</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1,2,3,4;5,6,7,8;9,10,11,12;13,14;15,16,17,18;19,20,21,22</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Rat_Offset_Effectivewin</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Mouse_TB_Ratio</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Reg4-4,Reg4-4o04,Reg4-4o5,Reg4-5,Reg4-6,Reg3-3,Reg3-3o03,Reg3-3o375,Reg3-3o75,Reg3-4o5</t>
+  </si>
+  <si>
+    <t>2001.9,2001.9,2001.9,2001.9,2001.9,2001.2,2001.2,2001.2,2001.2,2001.2</t>
+  </si>
+  <si>
+    <t>3000,3000,3000,3000,3000,3000,3000,3000,3000,3000</t>
+  </si>
+  <si>
+    <t>4,4,4,4,4,4,3,3,3,3,3</t>
+  </si>
+  <si>
+    <t>4,4.04,4.5,5,6,3,3.03,3.375,3.75,4.5</t>
+  </si>
+  <si>
+    <t>#AAAAAA,#000000, #0000FF, #FFA500 ,#FF0000</t>
+  </si>
+  <si>
+    <t>-300, 700</t>
+  </si>
+  <si>
+    <t>1,2,3,4,5;6,7,8,9,10</t>
+  </si>
+  <si>
+    <t>Mouse_Offset_DiffICI</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>E:\RatLinearArray\RatSounds\2022-12-20_RLA_Offset_2_128\</t>
+  </si>
+  <si>
+    <t>1ms,2ms,4ms,8ms,16ms,32ms,64ms,128ms, noise</t>
+  </si>
+  <si>
+    <t>2560,2560,2560,2560,2560,2560,2560,2560,2560</t>
+  </si>
+  <si>
+    <t>-3000,1000</t>
+  </si>
+  <si>
+    <t>-3000,-200_9:-500,0</t>
+  </si>
+  <si>
+    <t>1,2,4,8,16,32,64,128,8</t>
+  </si>
+  <si>
+    <t>1,2,3,4,5;5,6,7,8,9</t>
   </si>
 </sst>
 </file>
@@ -1598,7 +1832,7 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="2"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="2"/>
   </cellStyleXfs>
-  <cellXfs count="42">
+  <cellXfs count="52">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
@@ -1687,6 +1921,30 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="9" applyFont="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="2" xfId="9" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="9" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="1"/>
+    <xf numFmtId="49" fontId="6" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="0" borderId="2" xfId="4" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="2" xfId="4" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="0" borderId="2" xfId="4" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="0" borderId="2" xfId="4" applyNumberFormat="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="4"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="4" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="10">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
@@ -1976,11 +2234,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C23A6ACB-7C6B-4CD1-9AC1-822BCA547FA6}">
-  <dimension ref="A1:AA70"/>
+  <dimension ref="A1:AA81"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A65" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="Z69" sqref="Z69"/>
+    <sheetView tabSelected="1" topLeftCell="M1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A76" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="U80" sqref="U80:V81"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -6348,6 +6606,699 @@
       <c r="Z70" s="8"/>
       <c r="AA70" s="1"/>
     </row>
+    <row r="71" spans="1:27" ht="42.75" x14ac:dyDescent="0.2">
+      <c r="A71" s="1" t="s">
+        <v>378</v>
+      </c>
+      <c r="C71" s="4" t="s">
+        <v>380</v>
+      </c>
+      <c r="D71" s="4" t="s">
+        <v>381</v>
+      </c>
+      <c r="E71" s="4" t="s">
+        <v>382</v>
+      </c>
+      <c r="F71" s="1" t="s">
+        <v>235</v>
+      </c>
+      <c r="G71" s="1" t="s">
+        <v>235</v>
+      </c>
+      <c r="H71" s="4" t="s">
+        <v>235</v>
+      </c>
+      <c r="I71" s="1" t="s">
+        <v>235</v>
+      </c>
+      <c r="J71" s="4" t="s">
+        <v>383</v>
+      </c>
+      <c r="K71" s="4" t="s">
+        <v>383</v>
+      </c>
+      <c r="L71" t="s">
+        <v>384</v>
+      </c>
+      <c r="M71">
+        <v>0</v>
+      </c>
+      <c r="N71">
+        <v>6</v>
+      </c>
+      <c r="O71" s="1" t="s">
+        <v>235</v>
+      </c>
+      <c r="P71" s="6" t="s">
+        <v>385</v>
+      </c>
+      <c r="Q71" s="1" t="s">
+        <v>302</v>
+      </c>
+      <c r="R71" s="1" t="s">
+        <v>304</v>
+      </c>
+      <c r="S71" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="T71" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="U71" s="1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="72" spans="1:27" ht="57" x14ac:dyDescent="0.2">
+      <c r="A72" s="1" t="s">
+        <v>379</v>
+      </c>
+      <c r="C72" s="4" t="s">
+        <v>380</v>
+      </c>
+      <c r="D72" s="4" t="s">
+        <v>386</v>
+      </c>
+      <c r="E72" s="4" t="s">
+        <v>382</v>
+      </c>
+      <c r="F72" s="1" t="s">
+        <v>235</v>
+      </c>
+      <c r="G72" s="1" t="s">
+        <v>235</v>
+      </c>
+      <c r="H72" s="4" t="s">
+        <v>235</v>
+      </c>
+      <c r="I72" s="1" t="s">
+        <v>235</v>
+      </c>
+      <c r="J72" s="4" t="s">
+        <v>383</v>
+      </c>
+      <c r="K72" s="4" t="s">
+        <v>383</v>
+      </c>
+      <c r="L72" t="s">
+        <v>384</v>
+      </c>
+      <c r="M72">
+        <v>0</v>
+      </c>
+      <c r="N72">
+        <v>6</v>
+      </c>
+      <c r="O72" s="1" t="s">
+        <v>235</v>
+      </c>
+      <c r="P72" s="6" t="s">
+        <v>385</v>
+      </c>
+      <c r="Q72" s="1" t="s">
+        <v>302</v>
+      </c>
+      <c r="R72" s="1" t="s">
+        <v>304</v>
+      </c>
+      <c r="S72" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="T72" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="U72" s="1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="73" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="A73" s="1" t="s">
+        <v>387</v>
+      </c>
+      <c r="C73" s="4" t="s">
+        <v>388</v>
+      </c>
+      <c r="D73" s="4" t="s">
+        <v>389</v>
+      </c>
+      <c r="E73" s="4" t="s">
+        <v>390</v>
+      </c>
+      <c r="F73" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="G73" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="H73" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="I73" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="J73" s="4" t="s">
+        <v>391</v>
+      </c>
+      <c r="K73" s="4" t="s">
+        <v>391</v>
+      </c>
+      <c r="L73" s="1" t="s">
+        <v>392</v>
+      </c>
+      <c r="M73" s="4" t="s">
+        <v>262</v>
+      </c>
+      <c r="N73" s="4" t="s">
+        <v>204</v>
+      </c>
+      <c r="O73" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="P73">
+        <v>1</v>
+      </c>
+      <c r="Q73" s="1" t="s">
+        <v>302</v>
+      </c>
+      <c r="R73" s="1" t="s">
+        <v>304</v>
+      </c>
+      <c r="S73" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="T73" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="U73" s="1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="74" spans="1:27" ht="57" x14ac:dyDescent="0.2">
+      <c r="A74" s="1" t="s">
+        <v>393</v>
+      </c>
+      <c r="C74" s="4" t="s">
+        <v>394</v>
+      </c>
+      <c r="D74" s="4" t="s">
+        <v>395</v>
+      </c>
+      <c r="E74" s="4" t="s">
+        <v>395</v>
+      </c>
+      <c r="F74" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="G74" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="H74" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="I74" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="J74" s="4" t="s">
+        <v>396</v>
+      </c>
+      <c r="K74" s="4" t="s">
+        <v>396</v>
+      </c>
+      <c r="L74" t="s">
+        <v>397</v>
+      </c>
+      <c r="M74">
+        <v>0</v>
+      </c>
+      <c r="N74">
+        <v>6</v>
+      </c>
+      <c r="O74" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="P74" s="6" t="s">
+        <v>398</v>
+      </c>
+      <c r="Q74" s="1" t="s">
+        <v>302</v>
+      </c>
+      <c r="R74" s="1" t="s">
+        <v>304</v>
+      </c>
+      <c r="S74" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="T74" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="U74" s="1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="75" spans="1:27" ht="57" x14ac:dyDescent="0.2">
+      <c r="A75" s="1" t="s">
+        <v>402</v>
+      </c>
+      <c r="C75" s="4" t="s">
+        <v>399</v>
+      </c>
+      <c r="D75" s="4" t="s">
+        <v>395</v>
+      </c>
+      <c r="E75" s="4" t="s">
+        <v>395</v>
+      </c>
+      <c r="F75" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="G75" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="H75" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="I75" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="J75" s="4" t="s">
+        <v>396</v>
+      </c>
+      <c r="K75" s="4" t="s">
+        <v>396</v>
+      </c>
+      <c r="L75" t="s">
+        <v>400</v>
+      </c>
+      <c r="M75">
+        <v>0</v>
+      </c>
+      <c r="N75">
+        <v>6</v>
+      </c>
+      <c r="O75" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="P75" s="6" t="s">
+        <v>401</v>
+      </c>
+      <c r="Q75" s="1" t="s">
+        <v>302</v>
+      </c>
+      <c r="R75" s="1" t="s">
+        <v>304</v>
+      </c>
+      <c r="S75" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="T75" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="U75" s="1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="76" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="A76" s="1" t="s">
+        <v>403</v>
+      </c>
+      <c r="B76" s="5" t="s">
+        <v>89</v>
+      </c>
+      <c r="C76" s="3" t="s">
+        <v>404</v>
+      </c>
+      <c r="D76" s="4" t="s">
+        <v>405</v>
+      </c>
+      <c r="E76" s="4" t="s">
+        <v>405</v>
+      </c>
+      <c r="F76" s="1" t="s">
+        <v>406</v>
+      </c>
+      <c r="G76" s="1" t="s">
+        <v>406</v>
+      </c>
+      <c r="H76" s="4" t="s">
+        <v>407</v>
+      </c>
+      <c r="I76" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="J76" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="K76" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="L76" t="s">
+        <v>14</v>
+      </c>
+      <c r="M76" s="8">
+        <v>0</v>
+      </c>
+      <c r="N76" s="8">
+        <v>6</v>
+      </c>
+      <c r="O76" s="4" t="s">
+        <v>406</v>
+      </c>
+      <c r="P76" s="8" t="s">
+        <v>408</v>
+      </c>
+      <c r="Q76" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="R76" s="8">
+        <v>8</v>
+      </c>
+      <c r="S76" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="T76" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="U76" s="34" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="77" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="A77" s="1" t="s">
+        <v>422</v>
+      </c>
+      <c r="B77" s="4" t="s">
+        <v>100</v>
+      </c>
+      <c r="C77" s="3" t="s">
+        <v>409</v>
+      </c>
+      <c r="D77" s="4" t="s">
+        <v>410</v>
+      </c>
+      <c r="E77" s="4" t="s">
+        <v>410</v>
+      </c>
+      <c r="F77" s="1" t="s">
+        <v>406</v>
+      </c>
+      <c r="G77" s="1" t="s">
+        <v>406</v>
+      </c>
+      <c r="H77" s="1" t="s">
+        <v>406</v>
+      </c>
+      <c r="I77" s="1" t="s">
+        <v>406</v>
+      </c>
+      <c r="J77" s="4" t="s">
+        <v>185</v>
+      </c>
+      <c r="K77" s="4" t="s">
+        <v>185</v>
+      </c>
+      <c r="L77" s="40" t="s">
+        <v>411</v>
+      </c>
+      <c r="M77">
+        <v>0</v>
+      </c>
+      <c r="N77" s="8">
+        <v>6</v>
+      </c>
+      <c r="O77" s="4" t="s">
+        <v>406</v>
+      </c>
+      <c r="P77" s="8" t="s">
+        <v>75</v>
+      </c>
+      <c r="Q77" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="R77">
+        <v>8</v>
+      </c>
+      <c r="S77" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="T77" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="U77" s="34" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="78" spans="1:27" ht="28.5" x14ac:dyDescent="0.2">
+      <c r="A78" s="1" t="s">
+        <v>418</v>
+      </c>
+      <c r="B78" s="37"/>
+      <c r="C78" s="35" t="s">
+        <v>412</v>
+      </c>
+      <c r="D78" s="4" t="s">
+        <v>94</v>
+      </c>
+      <c r="E78" s="42" t="s">
+        <v>413</v>
+      </c>
+      <c r="F78" s="32" t="s">
+        <v>414</v>
+      </c>
+      <c r="G78" s="32" t="s">
+        <v>415</v>
+      </c>
+      <c r="H78" s="36" t="s">
+        <v>237</v>
+      </c>
+      <c r="I78" s="34" t="s">
+        <v>217</v>
+      </c>
+      <c r="J78" s="42" t="s">
+        <v>416</v>
+      </c>
+      <c r="K78" s="36" t="s">
+        <v>417</v>
+      </c>
+      <c r="L78" s="33" t="s">
+        <v>239</v>
+      </c>
+      <c r="M78" s="33">
+        <v>0</v>
+      </c>
+      <c r="N78" s="43">
+        <v>6</v>
+      </c>
+      <c r="O78" s="34" t="s">
+        <v>240</v>
+      </c>
+      <c r="P78" s="8" t="s">
+        <v>181</v>
+      </c>
+      <c r="Q78" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="R78">
+        <v>12</v>
+      </c>
+      <c r="S78" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="T78" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="U78" s="34" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="79" spans="1:27" ht="57" x14ac:dyDescent="0.2">
+      <c r="A79" s="1" t="s">
+        <v>419</v>
+      </c>
+      <c r="C79" s="4" t="s">
+        <v>420</v>
+      </c>
+      <c r="D79" s="4" t="s">
+        <v>395</v>
+      </c>
+      <c r="E79" s="4" t="s">
+        <v>395</v>
+      </c>
+      <c r="F79" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="G79" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="H79" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="I79" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="J79" s="4" t="s">
+        <v>396</v>
+      </c>
+      <c r="K79" s="4" t="s">
+        <v>396</v>
+      </c>
+      <c r="L79" t="s">
+        <v>400</v>
+      </c>
+      <c r="M79">
+        <v>0</v>
+      </c>
+      <c r="N79">
+        <v>6</v>
+      </c>
+      <c r="O79" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="P79" s="6" t="s">
+        <v>421</v>
+      </c>
+      <c r="Q79" s="1" t="s">
+        <v>302</v>
+      </c>
+      <c r="R79" s="1" t="s">
+        <v>304</v>
+      </c>
+      <c r="S79" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="T79" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="U79" s="1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="80" spans="1:27" ht="28.5" x14ac:dyDescent="0.2">
+      <c r="A80" s="18" t="s">
+        <v>423</v>
+      </c>
+      <c r="B80" s="44"/>
+      <c r="C80" s="20" t="s">
+        <v>424</v>
+      </c>
+      <c r="D80" s="20" t="s">
+        <v>425</v>
+      </c>
+      <c r="E80" s="20" t="s">
+        <v>426</v>
+      </c>
+      <c r="F80" s="18" t="s">
+        <v>214</v>
+      </c>
+      <c r="G80" s="18" t="s">
+        <v>215</v>
+      </c>
+      <c r="H80" s="20" t="s">
+        <v>216</v>
+      </c>
+      <c r="I80" s="18" t="s">
+        <v>217</v>
+      </c>
+      <c r="J80" s="20" t="s">
+        <v>427</v>
+      </c>
+      <c r="K80" s="20" t="s">
+        <v>428</v>
+      </c>
+      <c r="L80" s="40" t="s">
+        <v>429</v>
+      </c>
+      <c r="M80" s="44">
+        <v>0</v>
+      </c>
+      <c r="N80" s="44">
+        <v>6</v>
+      </c>
+      <c r="O80" s="18" t="s">
+        <v>214</v>
+      </c>
+      <c r="P80" s="44" t="s">
+        <v>431</v>
+      </c>
+      <c r="Q80" s="18" t="s">
+        <v>430</v>
+      </c>
+      <c r="R80" s="18" t="s">
+        <v>223</v>
+      </c>
+      <c r="S80" s="23" t="s">
+        <v>224</v>
+      </c>
+      <c r="T80" s="23" t="s">
+        <v>224</v>
+      </c>
+      <c r="U80" s="45" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="81" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A81" s="46" t="s">
+        <v>432</v>
+      </c>
+      <c r="B81" s="47" t="s">
+        <v>433</v>
+      </c>
+      <c r="C81" s="48" t="s">
+        <v>434</v>
+      </c>
+      <c r="D81" s="49" t="s">
+        <v>435</v>
+      </c>
+      <c r="E81" s="49" t="s">
+        <v>435</v>
+      </c>
+      <c r="F81" s="46" t="s">
+        <v>436</v>
+      </c>
+      <c r="G81" s="46" t="s">
+        <v>436</v>
+      </c>
+      <c r="H81" s="49" t="s">
+        <v>437</v>
+      </c>
+      <c r="I81" s="46" t="s">
+        <v>217</v>
+      </c>
+      <c r="J81" s="49" t="s">
+        <v>438</v>
+      </c>
+      <c r="K81" s="49" t="s">
+        <v>438</v>
+      </c>
+      <c r="L81" s="50" t="s">
+        <v>239</v>
+      </c>
+      <c r="M81" s="51">
+        <v>0</v>
+      </c>
+      <c r="N81" s="51">
+        <v>6</v>
+      </c>
+      <c r="O81" s="49" t="s">
+        <v>436</v>
+      </c>
+      <c r="P81" s="51" t="s">
+        <v>439</v>
+      </c>
+      <c r="Q81" s="46" t="s">
+        <v>222</v>
+      </c>
+      <c r="R81" s="18" t="s">
+        <v>223</v>
+      </c>
+      <c r="S81" s="51" t="s">
+        <v>224</v>
+      </c>
+      <c r="T81" s="51" t="s">
+        <v>224</v>
+      </c>
+      <c r="U81" s="34" t="s">
+        <v>241</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
update 2025-11-25 10:24:57 by win-g08qkcqo325
</commit_message>
<xml_diff>
--- a/config/RNP_CTLConfig.xlsx
+++ b/config/RNP_CTLConfig.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24334"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F871CFE6-0151-43E7-8CA5-B8E690D53062}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C63ACAE9-5AD6-4DBE-B1FC-DAA6E86741FE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15620" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="2" r:id="rId1"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1410" uniqueCount="440">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1447" uniqueCount="454">
   <si>
     <t>paradigm</t>
   </si>
@@ -1715,6 +1715,62 @@
   </si>
   <si>
     <t>1,2,3,4,5;5,6,7,8,9</t>
+  </si>
+  <si>
+    <t>SSA2</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>@MLA_PlotRasterLfp_Bao2</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Std-Reg3-3.8-Dev-Reg4-5,Std-Reg4-5-Dev-Reg3-3.8</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>0,0</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>14000,14000</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>-500,15000</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>0,14000</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>4,4</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>SSA1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Rest-3600,Rest-2400,Rest-1200,Rest-800,Rest-400</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1000,1000,1000,1000,1000</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>@MLA_PlotRasterLfp_BaoOffset2</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>-200,1200</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>7</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
 </file>
@@ -2234,38 +2290,38 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C23A6ACB-7C6B-4CD1-9AC1-822BCA547FA6}">
-  <dimension ref="A1:AA81"/>
+  <dimension ref="A1:AA83"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="M1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A76" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="U80" sqref="U80:V81"/>
+    <sheetView tabSelected="1" topLeftCell="M1" zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A79" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="O91" sqref="O91"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="50.375" style="1" customWidth="1"/>
-    <col min="2" max="2" width="52.125" style="1" customWidth="1"/>
-    <col min="3" max="3" width="67.625" style="4" customWidth="1"/>
+    <col min="1" max="1" width="50.33203125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="52.08203125" style="1" customWidth="1"/>
+    <col min="3" max="3" width="67.58203125" style="4" customWidth="1"/>
     <col min="4" max="4" width="43" style="4" customWidth="1"/>
     <col min="5" max="5" width="43.5" style="4" customWidth="1"/>
-    <col min="6" max="7" width="14.625" style="1" customWidth="1"/>
+    <col min="6" max="7" width="14.58203125" style="1" customWidth="1"/>
     <col min="8" max="8" width="20.75" style="4" customWidth="1"/>
-    <col min="9" max="9" width="18.625" style="1" customWidth="1"/>
+    <col min="9" max="9" width="18.58203125" style="1" customWidth="1"/>
     <col min="10" max="10" width="23" style="4" customWidth="1"/>
     <col min="11" max="11" width="23.5" style="4" customWidth="1"/>
-    <col min="12" max="12" width="87.875" customWidth="1"/>
-    <col min="13" max="13" width="9.625" customWidth="1"/>
+    <col min="12" max="12" width="87.83203125" customWidth="1"/>
+    <col min="13" max="13" width="9.58203125" customWidth="1"/>
     <col min="14" max="14" width="10.75" customWidth="1"/>
-    <col min="15" max="15" width="15.875" style="1" customWidth="1"/>
-    <col min="16" max="16" width="15.875" customWidth="1"/>
-    <col min="17" max="17" width="15.875" style="1" customWidth="1"/>
+    <col min="15" max="15" width="15.83203125" style="1" customWidth="1"/>
+    <col min="16" max="16" width="15.83203125" customWidth="1"/>
+    <col min="17" max="17" width="15.83203125" style="1" customWidth="1"/>
     <col min="18" max="18" width="15" style="1" customWidth="1"/>
     <col min="19" max="19" width="20" style="8" customWidth="1"/>
     <col min="20" max="20" width="13" style="8" customWidth="1"/>
-    <col min="21" max="21" width="31.125" style="1" customWidth="1"/>
+    <col min="21" max="21" width="31.08203125" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" s="14" customFormat="1" ht="28.5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:21" s="14" customFormat="1" ht="28" x14ac:dyDescent="0.3">
       <c r="A1" s="9" t="s">
         <v>0</v>
       </c>
@@ -2330,7 +2386,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="2" spans="1:21" s="14" customFormat="1" ht="71.25" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:21" s="14" customFormat="1" ht="70" x14ac:dyDescent="0.3">
       <c r="A2" s="16" t="s">
         <v>52</v>
       </c>
@@ -2361,7 +2417,7 @@
       </c>
       <c r="U2" s="12"/>
     </row>
-    <row r="3" spans="1:21" ht="28.5" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:21" ht="28" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>108</v>
       </c>
@@ -2426,7 +2482,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="4" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>130</v>
       </c>
@@ -2491,7 +2547,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="5" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
         <v>109</v>
       </c>
@@ -2556,7 +2612,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="6" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
         <v>131</v>
       </c>
@@ -2621,7 +2677,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="7" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
         <v>110</v>
       </c>
@@ -2686,7 +2742,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="8" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
         <v>132</v>
       </c>
@@ -2751,7 +2807,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="9" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
         <v>111</v>
       </c>
@@ -2816,7 +2872,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="10" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
         <v>112</v>
       </c>
@@ -2881,7 +2937,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="11" spans="1:21" ht="28.5" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:21" ht="28" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
         <v>39</v>
       </c>
@@ -2946,7 +3002,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="12" spans="1:21" ht="28.5" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A12" s="25" t="s">
         <v>104</v>
       </c>
@@ -3011,7 +3067,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="13" spans="1:21" ht="28.5" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:21" ht="28" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
         <v>44</v>
       </c>
@@ -3076,7 +3132,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="14" spans="1:21" ht="28.5" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:21" ht="28" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="s">
         <v>55</v>
       </c>
@@ -3141,7 +3197,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="15" spans="1:21" ht="28.5" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:21" ht="28" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="s">
         <v>99</v>
       </c>
@@ -3206,7 +3262,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="16" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A16" s="27" t="s">
         <v>137</v>
       </c>
@@ -3269,7 +3325,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="17" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A17" s="1" t="s">
         <v>140</v>
       </c>
@@ -3331,7 +3387,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="18" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A18" s="1" t="s">
         <v>141</v>
       </c>
@@ -3393,7 +3449,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="19" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A19" s="27" t="s">
         <v>142</v>
       </c>
@@ -3455,7 +3511,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="20" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A20" s="27" t="s">
         <v>143</v>
       </c>
@@ -3517,7 +3573,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="21" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A21" s="27" t="s">
         <v>164</v>
       </c>
@@ -3579,7 +3635,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="22" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A22" s="1" t="s">
         <v>165</v>
       </c>
@@ -3641,7 +3697,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="23" spans="1:21" ht="28.5" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:21" ht="28" x14ac:dyDescent="0.3">
       <c r="A23" s="27" t="s">
         <v>168</v>
       </c>
@@ -3703,7 +3759,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="24" spans="1:21" ht="28.5" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:21" ht="28" x14ac:dyDescent="0.3">
       <c r="A24" s="27" t="s">
         <v>172</v>
       </c>
@@ -3765,7 +3821,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="25" spans="1:21" ht="28.5" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:21" ht="28" x14ac:dyDescent="0.3">
       <c r="A25" s="27" t="s">
         <v>173</v>
       </c>
@@ -3827,7 +3883,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="26" spans="1:21" ht="28.5" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:21" ht="28" x14ac:dyDescent="0.3">
       <c r="A26" s="27" t="s">
         <v>174</v>
       </c>
@@ -3889,7 +3945,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="28" spans="1:21" s="31" customFormat="1" ht="28.5" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:21" s="31" customFormat="1" ht="28" x14ac:dyDescent="0.3">
       <c r="A28" s="28" t="s">
         <v>182</v>
       </c>
@@ -3952,7 +4008,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="29" spans="1:21" s="31" customFormat="1" ht="28.5" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:21" s="31" customFormat="1" ht="28" x14ac:dyDescent="0.3">
       <c r="A29" s="28" t="s">
         <v>187</v>
       </c>
@@ -4015,7 +4071,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="30" spans="1:21" s="31" customFormat="1" ht="28.5" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:21" s="31" customFormat="1" ht="28" x14ac:dyDescent="0.3">
       <c r="A30" s="28" t="s">
         <v>188</v>
       </c>
@@ -4078,7 +4134,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="31" spans="1:21" s="31" customFormat="1" ht="28.5" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:21" s="31" customFormat="1" ht="28" x14ac:dyDescent="0.3">
       <c r="A31" s="28" t="s">
         <v>189</v>
       </c>
@@ -4141,7 +4197,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="32" spans="1:21" s="31" customFormat="1" ht="28.5" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:21" s="31" customFormat="1" ht="28" x14ac:dyDescent="0.3">
       <c r="A32" s="28" t="s">
         <v>191</v>
       </c>
@@ -4204,7 +4260,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="33" spans="1:21" s="31" customFormat="1" ht="28.5" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:21" s="31" customFormat="1" ht="28" x14ac:dyDescent="0.3">
       <c r="A33" s="28" t="s">
         <v>190</v>
       </c>
@@ -4267,7 +4323,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="34" spans="1:21" s="31" customFormat="1" ht="28.5" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:21" s="31" customFormat="1" ht="28" x14ac:dyDescent="0.3">
       <c r="A34" s="28" t="s">
         <v>193</v>
       </c>
@@ -4330,7 +4386,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="35" spans="1:21" s="31" customFormat="1" ht="28.5" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:21" s="31" customFormat="1" ht="28" x14ac:dyDescent="0.3">
       <c r="A35" s="28" t="s">
         <v>199</v>
       </c>
@@ -4393,7 +4449,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="36" spans="1:21" s="31" customFormat="1" ht="28.5" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:21" s="31" customFormat="1" ht="28" x14ac:dyDescent="0.3">
       <c r="A36" s="28" t="s">
         <v>200</v>
       </c>
@@ -4456,7 +4512,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="37" spans="1:21" s="31" customFormat="1" ht="28.5" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:21" s="31" customFormat="1" ht="28" x14ac:dyDescent="0.3">
       <c r="A37" s="28" t="s">
         <v>201</v>
       </c>
@@ -4519,7 +4575,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="38" spans="1:21" s="31" customFormat="1" ht="28.5" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:21" s="31" customFormat="1" ht="28" x14ac:dyDescent="0.3">
       <c r="A38" s="28" t="s">
         <v>202</v>
       </c>
@@ -4582,7 +4638,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="39" spans="1:21" s="31" customFormat="1" ht="28.5" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:21" s="31" customFormat="1" ht="28" x14ac:dyDescent="0.3">
       <c r="A39" s="28" t="s">
         <v>203</v>
       </c>
@@ -4645,7 +4701,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="40" spans="1:21" s="31" customFormat="1" ht="28.5" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:21" s="31" customFormat="1" ht="28" x14ac:dyDescent="0.3">
       <c r="A40" s="28" t="s">
         <v>205</v>
       </c>
@@ -4708,7 +4764,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="41" spans="1:21" s="31" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:21" s="31" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A41" s="28" t="s">
         <v>245</v>
       </c>
@@ -4771,7 +4827,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="42" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A42" s="1" t="s">
         <v>206</v>
       </c>
@@ -4833,7 +4889,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="43" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A43" s="1" t="s">
         <v>244</v>
       </c>
@@ -4895,7 +4951,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="44" spans="1:21" ht="28.5" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:21" ht="28" x14ac:dyDescent="0.3">
       <c r="A44" s="1" t="s">
         <v>231</v>
       </c>
@@ -4957,7 +5013,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="45" spans="1:21" ht="28.5" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:21" ht="28" x14ac:dyDescent="0.3">
       <c r="A45" s="32" t="s">
         <v>243</v>
       </c>
@@ -5020,7 +5076,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="46" spans="1:21" ht="28.5" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:21" ht="28" x14ac:dyDescent="0.3">
       <c r="A46" s="1" t="s">
         <v>254</v>
       </c>
@@ -5082,7 +5138,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="47" spans="1:21" ht="28.5" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:21" ht="28" x14ac:dyDescent="0.3">
       <c r="A47" s="1" t="s">
         <v>255</v>
       </c>
@@ -5145,7 +5201,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="48" spans="1:21" ht="27.6" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:21" ht="27.65" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A48" s="1" t="s">
         <v>263</v>
       </c>
@@ -5207,7 +5263,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="49" spans="1:27" ht="28.5" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:27" ht="28" x14ac:dyDescent="0.3">
       <c r="A49" s="1" t="s">
         <v>273</v>
       </c>
@@ -5269,7 +5325,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="50" spans="1:27" ht="15" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:27" ht="14.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A50" s="1" t="s">
         <v>278</v>
       </c>
@@ -5332,7 +5388,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="51" spans="1:27" s="31" customFormat="1" ht="28.5" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:27" s="31" customFormat="1" ht="28" x14ac:dyDescent="0.3">
       <c r="A51" s="39" t="s">
         <v>289</v>
       </c>
@@ -5395,7 +5451,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="52" spans="1:27" s="31" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:27" s="31" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A52" s="28" t="s">
         <v>282</v>
       </c>
@@ -5458,7 +5514,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="53" spans="1:27" ht="42.75" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:27" ht="42" x14ac:dyDescent="0.3">
       <c r="A53" s="1" t="s">
         <v>295</v>
       </c>
@@ -5523,7 +5579,7 @@
       <c r="Z53" s="8"/>
       <c r="AA53" s="1"/>
     </row>
-    <row r="54" spans="1:27" ht="28.5" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:27" ht="28" x14ac:dyDescent="0.3">
       <c r="A54" s="1" t="s">
         <v>305</v>
       </c>
@@ -5586,7 +5642,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="55" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A55" s="1" t="s">
         <v>312</v>
       </c>
@@ -5651,7 +5707,7 @@
       <c r="Z55" s="8"/>
       <c r="AA55" s="1"/>
     </row>
-    <row r="56" spans="1:27" ht="28.5" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:27" ht="28" x14ac:dyDescent="0.3">
       <c r="A56" s="1" t="s">
         <v>313</v>
       </c>
@@ -5713,7 +5769,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="57" spans="1:27" s="31" customFormat="1" ht="28.5" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:27" s="31" customFormat="1" ht="28" x14ac:dyDescent="0.3">
       <c r="A57" s="1" t="s">
         <v>320</v>
       </c>
@@ -5776,7 +5832,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="58" spans="1:27" ht="42.75" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:27" ht="42" x14ac:dyDescent="0.3">
       <c r="A58" s="1" t="s">
         <v>325</v>
       </c>
@@ -5841,7 +5897,7 @@
       <c r="Z58" s="8"/>
       <c r="AA58" s="1"/>
     </row>
-    <row r="59" spans="1:27" ht="42.75" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:27" ht="42" x14ac:dyDescent="0.3">
       <c r="A59" s="1" t="s">
         <v>332</v>
       </c>
@@ -5906,7 +5962,7 @@
       <c r="Z59" s="8"/>
       <c r="AA59" s="1"/>
     </row>
-    <row r="60" spans="1:27" ht="28.5" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:27" ht="28" x14ac:dyDescent="0.3">
       <c r="A60" s="1" t="s">
         <v>336</v>
       </c>
@@ -5968,7 +6024,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="61" spans="1:27" ht="28.5" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:27" ht="28" x14ac:dyDescent="0.3">
       <c r="A61" s="1" t="s">
         <v>337</v>
       </c>
@@ -6030,7 +6086,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="62" spans="1:27" ht="28.5" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:27" ht="28" x14ac:dyDescent="0.3">
       <c r="A62" s="1" t="s">
         <v>343</v>
       </c>
@@ -6092,7 +6148,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="63" spans="1:27" ht="28.5" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:27" ht="28" x14ac:dyDescent="0.3">
       <c r="A63" s="1" t="s">
         <v>346</v>
       </c>
@@ -6154,7 +6210,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="64" spans="1:27" ht="28.5" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:27" ht="28" x14ac:dyDescent="0.3">
       <c r="A64" s="1" t="s">
         <v>348</v>
       </c>
@@ -6216,7 +6272,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="65" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A65" s="1" t="s">
         <v>351</v>
       </c>
@@ -6278,7 +6334,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="66" spans="1:27" ht="42.75" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:27" ht="42" x14ac:dyDescent="0.3">
       <c r="A66" s="1" t="s">
         <v>361</v>
       </c>
@@ -6343,7 +6399,7 @@
       <c r="Z66" s="8"/>
       <c r="AA66" s="1"/>
     </row>
-    <row r="67" spans="1:27" ht="71.25" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:27" ht="70" x14ac:dyDescent="0.3">
       <c r="A67" s="1" t="s">
         <v>372</v>
       </c>
@@ -6408,7 +6464,7 @@
       <c r="Z67" s="8"/>
       <c r="AA67" s="1"/>
     </row>
-    <row r="68" spans="1:27" ht="71.25" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:27" ht="70" x14ac:dyDescent="0.3">
       <c r="A68" s="1" t="s">
         <v>373</v>
       </c>
@@ -6473,7 +6529,7 @@
       <c r="Z68" s="8"/>
       <c r="AA68" s="1"/>
     </row>
-    <row r="69" spans="1:27" ht="71.25" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:27" ht="70" x14ac:dyDescent="0.3">
       <c r="A69" s="1" t="s">
         <v>375</v>
       </c>
@@ -6538,7 +6594,7 @@
       <c r="Z69" s="8"/>
       <c r="AA69" s="1"/>
     </row>
-    <row r="70" spans="1:27" ht="42.75" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:27" ht="42" x14ac:dyDescent="0.3">
       <c r="A70" s="41" t="s">
         <v>376</v>
       </c>
@@ -6606,7 +6662,7 @@
       <c r="Z70" s="8"/>
       <c r="AA70" s="1"/>
     </row>
-    <row r="71" spans="1:27" ht="42.75" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:27" ht="42" x14ac:dyDescent="0.3">
       <c r="A71" s="1" t="s">
         <v>378</v>
       </c>
@@ -6668,7 +6724,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="72" spans="1:27" ht="57" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:27" ht="56" x14ac:dyDescent="0.3">
       <c r="A72" s="1" t="s">
         <v>379</v>
       </c>
@@ -6730,7 +6786,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="73" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A73" s="1" t="s">
         <v>387</v>
       </c>
@@ -6792,7 +6848,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="74" spans="1:27" ht="57" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:27" ht="56" x14ac:dyDescent="0.3">
       <c r="A74" s="1" t="s">
         <v>393</v>
       </c>
@@ -6854,7 +6910,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="75" spans="1:27" ht="57" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:27" ht="56" x14ac:dyDescent="0.3">
       <c r="A75" s="1" t="s">
         <v>402</v>
       </c>
@@ -6916,7 +6972,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="76" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A76" s="1" t="s">
         <v>403</v>
       </c>
@@ -6981,7 +7037,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="77" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A77" s="1" t="s">
         <v>422</v>
       </c>
@@ -7046,7 +7102,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="78" spans="1:27" ht="28.5" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:27" ht="28" x14ac:dyDescent="0.3">
       <c r="A78" s="1" t="s">
         <v>418</v>
       </c>
@@ -7109,7 +7165,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="79" spans="1:27" ht="57" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:27" ht="56" x14ac:dyDescent="0.3">
       <c r="A79" s="1" t="s">
         <v>419</v>
       </c>
@@ -7171,7 +7227,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="80" spans="1:27" ht="28.5" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:27" ht="28" x14ac:dyDescent="0.3">
       <c r="A80" s="18" t="s">
         <v>423</v>
       </c>
@@ -7234,7 +7290,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="81" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A81" s="46" t="s">
         <v>432</v>
       </c>
@@ -7297,6 +7353,130 @@
       </c>
       <c r="U81" s="34" t="s">
         <v>241</v>
+      </c>
+    </row>
+    <row r="82" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A82" s="1" t="s">
+        <v>440</v>
+      </c>
+      <c r="C82" s="4" t="s">
+        <v>442</v>
+      </c>
+      <c r="D82" s="4" t="s">
+        <v>443</v>
+      </c>
+      <c r="E82" s="4" t="s">
+        <v>444</v>
+      </c>
+      <c r="F82" s="1" t="s">
+        <v>445</v>
+      </c>
+      <c r="G82" s="1" t="s">
+        <v>445</v>
+      </c>
+      <c r="H82" s="1" t="s">
+        <v>446</v>
+      </c>
+      <c r="I82" s="1" t="s">
+        <v>446</v>
+      </c>
+      <c r="J82" s="4" t="s">
+        <v>447</v>
+      </c>
+      <c r="K82" s="4" t="s">
+        <v>447</v>
+      </c>
+      <c r="L82" t="s">
+        <v>220</v>
+      </c>
+      <c r="M82">
+        <v>0</v>
+      </c>
+      <c r="N82" s="28">
+        <v>6</v>
+      </c>
+      <c r="O82" s="1" t="s">
+        <v>445</v>
+      </c>
+      <c r="P82" t="s">
+        <v>21</v>
+      </c>
+      <c r="Q82" s="1" t="s">
+        <v>445</v>
+      </c>
+      <c r="R82" s="1" t="s">
+        <v>223</v>
+      </c>
+      <c r="S82" s="8" t="s">
+        <v>224</v>
+      </c>
+      <c r="T82" s="8" t="s">
+        <v>224</v>
+      </c>
+      <c r="U82" s="28" t="s">
+        <v>441</v>
+      </c>
+    </row>
+    <row r="83" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A83" s="1" t="s">
+        <v>448</v>
+      </c>
+      <c r="C83" s="4" t="s">
+        <v>449</v>
+      </c>
+      <c r="D83" s="4" t="s">
+        <v>353</v>
+      </c>
+      <c r="E83" s="4" t="s">
+        <v>450</v>
+      </c>
+      <c r="F83" s="1" t="s">
+        <v>452</v>
+      </c>
+      <c r="G83" s="1" t="s">
+        <v>452</v>
+      </c>
+      <c r="H83" s="1" t="s">
+        <v>452</v>
+      </c>
+      <c r="I83" s="1" t="s">
+        <v>452</v>
+      </c>
+      <c r="J83" s="4" t="s">
+        <v>196</v>
+      </c>
+      <c r="K83" s="4" t="s">
+        <v>355</v>
+      </c>
+      <c r="L83" t="s">
+        <v>220</v>
+      </c>
+      <c r="M83">
+        <v>0</v>
+      </c>
+      <c r="N83" s="28" t="s">
+        <v>453</v>
+      </c>
+      <c r="O83" s="1" t="s">
+        <v>452</v>
+      </c>
+      <c r="P83" t="s">
+        <v>123</v>
+      </c>
+      <c r="Q83" s="1" t="s">
+        <v>452</v>
+      </c>
+      <c r="R83" s="1" t="s">
+        <v>223</v>
+      </c>
+      <c r="S83" s="8" t="s">
+        <v>224</v>
+      </c>
+      <c r="T83" s="8" t="s">
+        <v>224</v>
+      </c>
+      <c r="U83" s="28" t="s">
+        <v>451</v>
       </c>
     </row>
   </sheetData>

</xml_diff>